<commit_message>
update : generate mcq
</commit_message>
<xml_diff>
--- a/evaluation-service/Faqs.xlsx
+++ b/evaluation-service/Faqs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\piSpring\welcome-to-esprit\evaluation-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9162D8-D8C7-44D5-9183-86C841D79940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0FDA8B-AACF-4E0A-ACBB-955AE2CDAF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
-  <si>
-    <t>a</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>admission</t>
   </si>
@@ -36,10 +33,19 @@
     <t>rules</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>payment</t>
+  </si>
+  <si>
+    <t>faq1e</t>
+  </si>
+  <si>
+    <t>resp1e</t>
+  </si>
+  <si>
+    <t>res2e</t>
+  </si>
+  <si>
+    <t>faq2e</t>
   </si>
 </sst>
 </file>
@@ -360,37 +366,37 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix : complete spring batch / add : aop
</commit_message>
<xml_diff>
--- a/evaluation-service/Faqs.xlsx
+++ b/evaluation-service/Faqs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\piSpring\welcome-to-esprit\evaluation-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0FDA8B-AACF-4E0A-ACBB-955AE2CDAF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE550D20-43B1-4690-B2AE-DB1AF1FF8EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>admission</t>
   </si>
@@ -36,16 +36,34 @@
     <t>payment</t>
   </si>
   <si>
-    <t>faq1e</t>
-  </si>
-  <si>
-    <t>resp1e</t>
-  </si>
-  <si>
-    <t>res2e</t>
-  </si>
-  <si>
-    <t>faq2e</t>
+    <t>What programs do you offer?</t>
+  </si>
+  <si>
+    <t>We offer a wide range of undergraduate and graduate programs in various fields, including engineering, computer science, business, and law. You can find more information about our programs on our website, or by contacting our admissions office.</t>
+  </si>
+  <si>
+    <t>How do I apply for admission?</t>
+  </si>
+  <si>
+    <t>You can apply for admission online through our website. Simply select the program you are interested in, and follow the instructions provided. You will need to submit your academic transcripts, test scores, and other required documents along with your application.</t>
+  </si>
+  <si>
+    <t>What are the admission requirements?</t>
+  </si>
+  <si>
+    <t>Admission requirements vary by program, but generally include a minimum GPA, standardized test scores (such as the SAT or ACT), and letters of recommendation. Specific requirements can be found on our website, or by contacting our admissions office.</t>
+  </si>
+  <si>
+    <t>What financial aid options are available?</t>
+  </si>
+  <si>
+    <t>We offer a variety of financial aid options, including scholarships, grants, loans, and work-study programs. You can find more information about financial aid on our website, or by contacting our financial aid office.</t>
+  </si>
+  <si>
+    <t>How can I schedule a campus visit?</t>
+  </si>
+  <si>
+    <t>You can schedule a campus visit through our website, or by contacting our admissions office. Campus visits typically include a tour of our facilities, meetings with faculty and staff, and the opportunity to attend a class or event.</t>
   </si>
 </sst>
 </file>
@@ -363,13 +381,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="52" customWidth="1"/>
+    <col min="2" max="2" width="97.21875" customWidth="1"/>
+    <col min="3" max="3" width="54.44140625" customWidth="1"/>
+    <col min="4" max="4" width="43.33203125" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -390,13 +415,37 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>